<commit_message>
Improve integration of pathways
</commit_message>
<xml_diff>
--- a/CASPIANII/ListeNeobiota/Data/Input/PfadUebersetzung.xlsx
+++ b/CASPIANII/ListeNeobiota/Data/Input/PfadUebersetzung.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hanno\Bioinvasion\CASPIANII\CASPIANII\ListeNeobiota\Data\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>CASPIAN</t>
   </si>
@@ -103,24 +108,6 @@
     <t>als blinder Passagier der Bahn</t>
   </si>
   <si>
-    <t>Container/bulk</t>
-  </si>
-  <si>
-    <t>TRANSPORT.-.STOWAWAY:.Container./.bulk</t>
-  </si>
-  <si>
-    <t>Transport über Holzpaletten</t>
-  </si>
-  <si>
-    <t>Organic packing material</t>
-  </si>
-  <si>
-    <t>TRANSPORT.-.STOWAWAY:.Organic.packing.material,.in.particular.wood.packaging</t>
-  </si>
-  <si>
-    <t>Andere Gütertransporte</t>
-  </si>
-  <si>
     <t>mit Saatgut oder Futtermitteln</t>
   </si>
   <si>
@@ -158,9 +145,6 @@
   </si>
   <si>
     <t>TRANSPORT.-.STOWAWAY:.Angling/fishing.equipment; TRANSPORT.-.STOWAWAY:.People.and.their.luggage/equipment.(in.particular.tourism)</t>
-  </si>
-  <si>
-    <t>Absichtlich</t>
   </si>
   <si>
     <t>Jagd; Ansalbung; Fischerei; Forstwirtschaft; Gartenbau; Landschaftsbau; Private Einfuhr; Naturschutzmaßnahme; Biologische Kontrolle</t>
@@ -241,9 +225,6 @@
     <t>CORRIDOR:.Interconnected.waterways/basins/seas; CORRIDOR:.Tunnels.and.land.bridges</t>
   </si>
   <si>
-    <t>Andere Pfade</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -348,11 +329,30 @@
   <si>
     <t>Anhaftung an Landfahrzeuge</t>
   </si>
+  <si>
+    <t>absichtlich</t>
+  </si>
+  <si>
+    <t>andere Gütertransporte</t>
+  </si>
+  <si>
+    <t>andere Pfade</t>
+  </si>
+  <si>
+    <t>unbekannt</t>
+  </si>
+  <si>
+    <t>TRANSPORT.-.STOWAWAY:.Container./.bulk; 
+TRANSPORT.-.STOWAWAY:.Organic.packing.material,.in.particular.wood.packaging</t>
+  </si>
+  <si>
+    <t>Container/bulk; Organic packing material</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -418,14 +418,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -463,9 +466,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +503,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,7 +538,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -709,25 +712,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="41.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" style="2" customWidth="1"/>
     <col min="4" max="4" width="41" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="99.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" style="2" customWidth="1"/>
-    <col min="8" max="1024" width="11.5703125" style="2"/>
+    <col min="5" max="5" width="22.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="106.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="54.453125" style="2" customWidth="1"/>
+    <col min="8" max="1024" width="11.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,63 +751,63 @@
       </c>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="50.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -820,25 +823,25 @@
       </c>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -856,7 +859,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -874,9 +877,9 @@
       </c>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -892,25 +895,25 @@
       </c>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -919,43 +922,43 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" ht="141" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="126" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" ht="54" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:7" ht="70.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -963,17 +966,17 @@
         <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -988,65 +991,50 @@
       </c>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>86</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>67</v>
-      </c>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G26"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G27"/>
     </row>
   </sheetData>
   <sortState ref="A2:AMJ27">
@@ -1069,444 +1057,444 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E62" s="5"/>
     </row>
-    <row r="63" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" s="4"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" s="4"/>
     </row>
-    <row r="70" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E70" s="5"/>
     </row>
-    <row r="71" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E71" s="5"/>
     </row>
-    <row r="72" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E73" s="5"/>
     </row>
-    <row r="74" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E74" s="5"/>
     </row>
-    <row r="75" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E75" s="5"/>
     </row>
-    <row r="76" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E76" s="5"/>
     </row>
-    <row r="77" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E77" s="5"/>
     </row>
-    <row r="78" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E79" s="5"/>
     </row>
-    <row r="80" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E80" s="5"/>
     </row>
-    <row r="81" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E82" s="5"/>
     </row>
-    <row r="83" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E83" s="5"/>
     </row>
-    <row r="84" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E84" s="5"/>
     </row>
-    <row r="85" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E85" s="5"/>
     </row>
-    <row r="86" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E86" s="5"/>
     </row>
-    <row r="87" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E87" s="5"/>
     </row>
-    <row r="88" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E88" s="5"/>
     </row>
-    <row r="89" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E89" s="5"/>
     </row>
-    <row r="90" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E90" s="5"/>
     </row>
-    <row r="91" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E91" s="5"/>
     </row>
-    <row r="92" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E92" s="5"/>
     </row>
-    <row r="93" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E93" s="5"/>
     </row>
-    <row r="94" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E94" s="5"/>
     </row>
-    <row r="95" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E95" s="5"/>
     </row>
-    <row r="96" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E96" s="5"/>
     </row>
-    <row r="97" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E97" s="5"/>
     </row>
-    <row r="98" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E98" s="5"/>
     </row>
-    <row r="99" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E99" s="5"/>
     </row>
-    <row r="100" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E100" s="5"/>
     </row>
-    <row r="101" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E101" s="5"/>
     </row>
-    <row r="102" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E102" s="5"/>
     </row>
-    <row r="103" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E103" s="5"/>
     </row>
-    <row r="104" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E104" s="5"/>
     </row>
-    <row r="105" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E105" s="5"/>
     </row>
-    <row r="106" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E106" s="5"/>
     </row>
-    <row r="107" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E107" s="5"/>
     </row>
-    <row r="108" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E108" s="5"/>
     </row>
-    <row r="109" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E109" s="5"/>
     </row>
-    <row r="110" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E110" s="5"/>
     </row>
-    <row r="111" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E111" s="5"/>
     </row>
-    <row r="112" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E112" s="5"/>
     </row>
-    <row r="113" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E113" s="5"/>
     </row>
-    <row r="114" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E114" s="5"/>
     </row>
-    <row r="115" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E115" s="5"/>
     </row>
-    <row r="116" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E116" s="5"/>
     </row>
-    <row r="117" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E117" s="5"/>
     </row>
-    <row r="118" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E118" s="5"/>
     </row>
-    <row r="119" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E119" s="5"/>
     </row>
-    <row r="120" spans="5:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E120" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version of NaVI app
Added BfN species lists
Adjusted mouse over
Added major species groups in tables

Several minor improvements
</commit_message>
<xml_diff>
--- a/CASPIANII/ListeNeobiota/Data/Input/PfadUebersetzung.xlsx
+++ b/CASPIANII/ListeNeobiota/Data/Input/PfadUebersetzung.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
     <t>CASPIAN</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>Container/bulk; Organic packing material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport - Contaminant; Transport - Contaminant &amp; Stowaway </t>
   </si>
 </sst>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -724,7 +727,7 @@
     <col min="2" max="2" width="34.453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="29.453125" style="2" customWidth="1"/>
     <col min="4" max="4" width="41" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" style="2" customWidth="1"/>
     <col min="6" max="6" width="106.7265625" style="2" customWidth="1"/>
     <col min="7" max="7" width="54.453125" style="2" customWidth="1"/>
     <col min="8" max="1024" width="11.54296875" style="2"/>
@@ -783,7 +786,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>31</v>
@@ -1041,7 +1044,7 @@
     <sortCondition ref="A2:A27"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>